<commit_message>
bug fixed, added mean difference tests
</commit_message>
<xml_diff>
--- a/Organization/projects_stats.xlsx
+++ b/Organization/projects_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepp_\SpyderWorkspace\Commit_Analysis\developersBreaksAnalysis\Organization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03E1209-354E-4A77-BF0E-2CB063A562D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB13C97A-8B88-4185-8CBD-5EEF06F554A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="-9990" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projects_stats" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Contributors</t>
-  </si>
-  <si>
-    <t>Sampled_Contributors</t>
   </si>
   <si>
     <t>rails</t>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>Gone</t>
+  </si>
+  <si>
+    <t>Core developers</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Sampled_Contributors</c:v>
+                  <c:v>Core developers</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2340,7 +2340,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C20" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2353,21 +2353,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>3834</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1979</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>851</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>765</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>431</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>402</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>331</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>204</v>

</xml_diff>